<commit_message>
v750 update - minor bug fixed with angle curve in pipeline
</commit_message>
<xml_diff>
--- a/examples/ex051.MF_pipeline.xlsx
+++ b/examples/ex051.MF_pipeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unifloc\unifloc_vba\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\unifloc\unifloc_vba\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE015496-0D54-4971-A679-0DEC0317C57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1308DFC7-C0B6-4296-81F5-50D9E8D23A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{52E28BDD-AE60-49A1-BCFC-DEAA796E2D5C}"/>
+    <workbookView xWindow="780" yWindow="-20820" windowWidth="31530" windowHeight="19905" xr2:uid="{52E28BDD-AE60-49A1-BCFC-DEAA796E2D5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,10 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
+    <definedName name="feed_json">Лист1!$I$58</definedName>
     <definedName name="pipe_construction">Лист1!$Q$4</definedName>
     <definedName name="pipe_object">Лист1!$S$31</definedName>
+    <definedName name="PVT_json">Лист1!$I$53</definedName>
     <definedName name="t_model">Лист1!$Q$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -35,8 +37,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>trajectory</t>
   </si>
@@ -146,6 +146,36 @@
   </si>
   <si>
     <t>4. Запустить пример расчета распределения давления и температуры в трубе</t>
+  </si>
+  <si>
+    <t>gamma_gas</t>
+  </si>
+  <si>
+    <t>gamma_oil</t>
+  </si>
+  <si>
+    <t>gamma_wat</t>
+  </si>
+  <si>
+    <t>rsb_m3m3</t>
+  </si>
+  <si>
+    <t>pb_atma</t>
+  </si>
+  <si>
+    <t>t_res_C</t>
+  </si>
+  <si>
+    <t>bob_m3m3</t>
+  </si>
+  <si>
+    <t>muob_cP</t>
+  </si>
+  <si>
+    <t>pvt_corr_set</t>
+  </si>
+  <si>
+    <t>PVT</t>
   </si>
 </sst>
 </file>
@@ -332,64 +362,64 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.382340650400337</c:v>
+                  <c:v>24.836360057558057</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48.369222249982833</c:v>
+                  <c:v>39.660912169855287</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60.235098269119753</c:v>
+                  <c:v>54.473728023011631</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>64.947911242525024</c:v>
+                  <c:v>69.274877304399666</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72.00729056417785</c:v>
+                  <c:v>84.064262054326051</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>83.666494542562518</c:v>
+                  <c:v>98.841955005012849</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>95.192463420676702</c:v>
+                  <c:v>113.60819486374973</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>106.10446404258369</c:v>
+                  <c:v>128.36305394047776</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>116.24710999851564</c:v>
+                  <c:v>143.10660666796306</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>126.27329543079401</c:v>
+                  <c:v>157.83860705561924</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>136.18755283448164</c:v>
+                  <c:v>172.55946291726846</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>145.9943761710272</c:v>
+                  <c:v>187.26925720901431</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>155.69830991372984</c:v>
+                  <c:v>201.96807608679808</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>165.28460789209592</c:v>
+                  <c:v>216.65585276159905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>174.0541851495523</c:v>
+                  <c:v>231.33268489206455</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>176.40915429020524</c:v>
+                  <c:v>233.09334496046432</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>182.44123403347325</c:v>
+                  <c:v>245.98725456824823</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>190.77003183492977</c:v>
+                  <c:v>260.62969555631469</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>199.04259166672151</c:v>
+                  <c:v>275.2616896761848</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -404,58 +434,58 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>147.05882352941177</c:v>
+                  <c:v>138.88888888888889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>294.11764705882354</c:v>
+                  <c:v>277.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>441.1764705882353</c:v>
+                  <c:v>416.66666666666663</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500</c:v>
+                  <c:v>555.55555555555554</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>588.23529411764707</c:v>
+                  <c:v>694.44444444444446</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>735.29411764705878</c:v>
+                  <c:v>833.33333333333326</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>882.35294117647061</c:v>
+                  <c:v>972.22222222222217</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1029.4117647058824</c:v>
+                  <c:v>1111.1111111111111</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1176.4705882352941</c:v>
+                  <c:v>1250</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1323.5294117647059</c:v>
+                  <c:v>1388.8888888888889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1470.5882352941176</c:v>
+                  <c:v>1527.7777777777778</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1617.6470588235295</c:v>
+                  <c:v>1666.6666666666665</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1764.7058823529412</c:v>
+                  <c:v>1805.5555555555554</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1911.7647058823529</c:v>
+                  <c:v>1944.4444444444443</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2058.8235294117649</c:v>
+                  <c:v>2083.3333333333335</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2205.8823529411766</c:v>
+                  <c:v>2222.2222222222222</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2352.9411764705883</c:v>
+                  <c:v>2361.1111111111109</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2500</c:v>
@@ -913,61 +943,61 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.676470588235293</c:v>
+                  <c:v>12.666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.352941176470587</c:v>
+                  <c:v>15.333333333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.029411764705884</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.5</c:v>
+                  <c:v>20.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.705882352941178</c:v>
+                  <c:v>23.333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.382352941176471</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32.058823529411768</c:v>
+                  <c:v>28.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.191176470588239</c:v>
+                  <c:v>31.333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42.147058823529413</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>48.102941176470587</c:v>
+                  <c:v>36.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>54.058823529411761</c:v>
+                  <c:v>39.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60.014705882352942</c:v>
+                  <c:v>41.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65.970588235294116</c:v>
+                  <c:v>44.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>71.92647058823529</c:v>
+                  <c:v>47.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>77.617647058823536</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>79.099999999999994</c:v>
+                  <c:v>50.319999999999993</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>81.294117647058826</c:v>
+                  <c:v>52.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>83.647058823529406</c:v>
+                  <c:v>55.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>86</c:v>
+                  <c:v>57.999999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -982,61 +1012,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>147.05882352941177</c:v>
+                  <c:v>138.88888888888889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>294.11764705882354</c:v>
+                  <c:v>277.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>441.1764705882353</c:v>
+                  <c:v>416.66666666666663</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500</c:v>
+                  <c:v>555.55555555555554</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>588.23529411764707</c:v>
+                  <c:v>694.44444444444446</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>735.29411764705878</c:v>
+                  <c:v>833.33333333333326</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>882.35294117647061</c:v>
+                  <c:v>972.22222222222217</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1026.4705882352941</c:v>
+                  <c:v>1111.1111111111111</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1158.8235294117646</c:v>
+                  <c:v>1250</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1291.1764705882354</c:v>
+                  <c:v>1388.8888888888889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1423.5294117647059</c:v>
+                  <c:v>1527.7777777777778</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1555.8823529411766</c:v>
+                  <c:v>1666.6666666666665</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1688.2352941176471</c:v>
+                  <c:v>1805.5555555555554</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1820.5882352941176</c:v>
+                  <c:v>1944.4444444444443</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1947.0588235294119</c:v>
+                  <c:v>2083.3333333333335</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1980</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2064.7058823529414</c:v>
+                  <c:v>2222.2222222222222</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2182.3529411764707</c:v>
+                  <c:v>2361.1111111111109</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2300</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1088,61 +1118,61 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.676470588235293</c:v>
+                  <c:v>12.666666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.352941176470587</c:v>
+                  <c:v>15.333333333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.029411764705884</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.5</c:v>
+                  <c:v>20.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.705882352941178</c:v>
+                  <c:v>23.333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.382352941176471</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32.058823529411768</c:v>
+                  <c:v>28.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.191176470588239</c:v>
+                  <c:v>31.333333333333332</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42.147058823529413</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>48.102941176470587</c:v>
+                  <c:v>36.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>54.058823529411761</c:v>
+                  <c:v>39.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60.014705882352942</c:v>
+                  <c:v>41.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65.970588235294116</c:v>
+                  <c:v>44.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>71.92647058823529</c:v>
+                  <c:v>47.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>77.617647058823536</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>79.099999999999994</c:v>
+                  <c:v>50.319999999999993</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>81.294117647058826</c:v>
+                  <c:v>52.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>83.647058823529406</c:v>
+                  <c:v>55.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>86</c:v>
+                  <c:v>57.999999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1157,61 +1187,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>147.05882352941177</c:v>
+                  <c:v>138.88888888888889</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>294.11764705882354</c:v>
+                  <c:v>277.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>441.1764705882353</c:v>
+                  <c:v>416.66666666666663</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500</c:v>
+                  <c:v>555.55555555555554</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>588.23529411764707</c:v>
+                  <c:v>694.44444444444446</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>735.29411764705878</c:v>
+                  <c:v>833.33333333333326</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>882.35294117647061</c:v>
+                  <c:v>972.22222222222217</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1026.4705882352941</c:v>
+                  <c:v>1111.1111111111111</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1158.8235294117646</c:v>
+                  <c:v>1250</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1291.1764705882354</c:v>
+                  <c:v>1388.8888888888889</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1423.5294117647059</c:v>
+                  <c:v>1527.7777777777778</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1555.8823529411766</c:v>
+                  <c:v>1666.6666666666665</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1688.2352941176471</c:v>
+                  <c:v>1805.5555555555554</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1820.5882352941176</c:v>
+                  <c:v>1944.4444444444443</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1947.0588235294119</c:v>
+                  <c:v>2083.3333333333335</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1980</c:v>
+                  <c:v>2100</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2064.7058823529414</c:v>
+                  <c:v>2222.2222222222222</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2182.3529411764707</c:v>
+                  <c:v>2361.1111111111109</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2300</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3290,11 +3320,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Info"/>
     </sheetNames>
@@ -3302,6 +3329,7 @@
       <definedName name="encode_feed"/>
       <definedName name="encode_pipe"/>
       <definedName name="encode_pipe_construction"/>
+      <definedName name="encode_PVT"/>
       <definedName name="encode_t_model"/>
       <definedName name="MF_pipe_p_atma"/>
     </definedNames>
@@ -3609,36 +3637,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B18ED9F-76C8-4FA4-B5AD-788BF17B54D3}">
+  <sheetPr codeName="Лист1"/>
   <dimension ref="B1:Y66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Q4" s="3" t="str">
         <f>[1]!encode_pipe_construction(P7:Q10,R7:S10)</f>
-        <v>{"h_list_m":{"hmes_m":[0,1000,2000,2500],"hvert_m":[0,1000,1900,2300]},"diam_list_mm":{"hmes_m":[0,500,2100,2500],"diam_int_mm":[62,72,125,125]}}</v>
+        <v>{"h_list_m":{"hmes_m":[0,1000,2000,2500],"hvert_m":[0,1000,2000,2500]},"diam_list_mm":{"hmes_m":[0,500,2100,2500],"diam_int_mm":[62,62,125,125]}}</v>
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P5" s="1" t="s">
         <v>0</v>
       </c>
@@ -3648,7 +3677,7 @@
       </c>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P6" s="1" t="s">
         <v>2</v>
       </c>
@@ -3662,7 +3691,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P7" s="2">
         <v>0</v>
       </c>
@@ -3676,7 +3705,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P8" s="2">
         <v>1000</v>
       </c>
@@ -3687,15 +3716,15 @@
         <v>500</v>
       </c>
       <c r="S8" s="4">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P9" s="2">
         <v>2000</v>
       </c>
       <c r="Q9" s="2">
-        <v>1900</v>
+        <v>2000</v>
       </c>
       <c r="R9" s="4">
         <v>2100</v>
@@ -3704,37 +3733,37 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P10" s="2">
         <v>2500</v>
       </c>
       <c r="Q10" s="2">
-        <v>2300</v>
+        <v>2500</v>
       </c>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="Q13" s="3" t="str">
         <f>[1]!encode_t_model(1,P16:Q19)</f>
-        <v>{"t_model":1,"t_list_C":{"hvert_m":[0,1000,2000,2500],"t_C":[10,35,80,90]}}</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
+        <v>{"t_model":1,"t_list_C":{"hvert_m":[0,2500],"t_C":[10,58]}}</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P15" s="1" t="s">
         <v>3</v>
       </c>
@@ -3742,7 +3771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P16" s="2">
         <v>0</v>
       </c>
@@ -3750,54 +3779,46 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="P17" s="2">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="Q17" s="2">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="P18" s="2">
-        <v>2000</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="P19" s="2">
-        <v>2500</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="R22" s="1" t="s">
         <v>5</v>
       </c>
       <c r="S22" s="5" t="str">
         <f>pipe_construction</f>
-        <v>{"h_list_m":{"hmes_m":[0,1000,2000,2500],"hvert_m":[0,1000,1900,2300]},"diam_list_mm":{"hmes_m":[0,500,2100,2500],"diam_int_mm":[62,72,125,125]}}</v>
-      </c>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.35">
+        <v>{"h_list_m":{"hmes_m":[0,1000,2000,2500],"hvert_m":[0,1000,2000,2500]},"diam_list_mm":{"hmes_m":[0,500,2100,2500],"diam_int_mm":[62,62,125,125]}}</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="R23" s="1" t="s">
         <v>9</v>
       </c>
       <c r="S23" s="5" t="str">
         <f>t_model</f>
-        <v>{"t_model":1,"t_list_C":{"hvert_m":[0,1000,2000,2500],"t_C":[10,35,80,90]}}</v>
-      </c>
-    </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.35">
+        <v>{"t_model":1,"t_list_C":{"hvert_m":[0,2500],"t_C":[10,58]}}</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="R24" s="1" t="s">
         <v>10</v>
       </c>
@@ -3805,7 +3826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="R25" s="1" t="s">
         <v>11</v>
       </c>
@@ -3813,7 +3834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="R26" s="1" t="s">
         <v>12</v>
       </c>
@@ -3821,7 +3842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
       <c r="R27" s="1" t="s">
         <v>13</v>
       </c>
@@ -3829,25 +3850,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
       <c r="R28" s="1" t="s">
         <v>14</v>
       </c>
       <c r="S28" s="2"/>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="R29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="S29" s="2"/>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="R30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="S30" s="2"/>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>33</v>
       </c>
@@ -3856,18 +3877,18 @@
       </c>
       <c r="S31" s="3" t="str">
         <f>[1]!encode_pipe(S22,S23,S24,S25,S26,S27,S28,S29,S30)</f>
-        <v>{"construction":{"h_list_m":{"hmes_m":[0,1000,2000,2500],"hvert_m":[0,1000,1900,2300]},"diam_list_mm":{"hmes_m":[0,500,2100,2500],"diam_int_mm":[62,72,125,125]}},"t_model":{"t_model":1,"t_list_C":{"hvert_m":[0,1000,2000,2500],"t_C":[10,35,80,90]}},"flow_correlation":0,"flow_along_coord":false,"calibr_grav":1,"calibr_fric":1,"h_start_m":0,"h_end_m":0,"znlf":false}</v>
-      </c>
-    </row>
-    <row r="34" spans="18:25" x14ac:dyDescent="0.35">
+        <v>{"construction":{"h_list_m":{"hmes_m":[0,1000,2000,2500],"hvert_m":[0,1000,2000,2500]},"diam_list_mm":{"hmes_m":[0,500,2100,2500],"diam_int_mm":[62,62,125,125]}},"t_model":{"t_model":1,"t_list_C":{"hvert_m":[0,2500],"t_C":[10,58]}},"flow_correlation":0,"flow_along_coord":false,"calibr_grav":1,"calibr_fric":1,"h_start_m":0,"h_end_m":0,"znlf":false}</v>
+      </c>
+    </row>
+    <row r="34" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R34" s="1" t="s">
         <v>18</v>
       </c>
       <c r="S34" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="18:25" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R35" s="1" t="s">
         <v>19</v>
       </c>
@@ -3875,25 +3896,25 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="36" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R36" s="1" t="s">
         <v>20</v>
       </c>
       <c r="S36" s="5" t="str">
         <f>pipe_object</f>
-        <v>{"construction":{"h_list_m":{"hmes_m":[0,1000,2000,2500],"hvert_m":[0,1000,1900,2300]},"diam_list_mm":{"hmes_m":[0,500,2100,2500],"diam_int_mm":[62,72,125,125]}},"t_model":{"t_model":1,"t_list_C":{"hvert_m":[0,1000,2000,2500],"t_C":[10,35,80,90]}},"flow_correlation":0,"flow_along_coord":false,"calibr_grav":1,"calibr_fric":1,"h_start_m":0,"h_end_m":0,"znlf":false}</v>
-      </c>
-    </row>
-    <row r="37" spans="18:25" x14ac:dyDescent="0.35">
+        <v>{"construction":{"h_list_m":{"hmes_m":[0,1000,2000,2500],"hvert_m":[0,1000,2000,2500]},"diam_list_mm":{"hmes_m":[0,500,2100,2500],"diam_int_mm":[62,62,125,125]}},"t_model":{"t_model":1,"t_list_C":{"hvert_m":[0,2500],"t_C":[10,58]}},"flow_correlation":0,"flow_along_coord":false,"calibr_grav":1,"calibr_fric":1,"h_start_m":0,"h_end_m":0,"znlf":false}</v>
+      </c>
+    </row>
+    <row r="37" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R37" s="1" t="s">
         <v>21</v>
       </c>
       <c r="S37" s="5" t="str">
-        <f>[1]!encode_feed()</f>
-        <v>{"gamma_gas":0.6,"gamma_oil":0.86,"gamma_wat":1,"rsb_m3m3":100,"q_liq_sm3day":10}</v>
-      </c>
-    </row>
-    <row r="38" spans="18:25" x14ac:dyDescent="0.35">
+        <f>feed_json</f>
+        <v>{"gamma_gas":0.6,"gamma_oil":0.86,"gamma_wat":1.1,"rsb_m3m3":120,"pb_atma":130,"t_res_C":80,"bob_m3m3":1.2,"muob_cP":0.6,"PVT_corr_set":0,"q_liq_sm3day":50,"fw_perc":100,"rp_m3m3":120}</v>
+      </c>
+    </row>
+    <row r="38" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R38" s="1" t="s">
         <v>22</v>
       </c>
@@ -3901,7 +3922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="39" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R39" s="1" t="s">
         <v>23</v>
       </c>
@@ -3909,46 +3930,52 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="40" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R40" s="1" t="s">
         <v>25</v>
       </c>
       <c r="S40" s="2"/>
     </row>
-    <row r="41" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="41" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R41" s="1" t="s">
         <v>26</v>
       </c>
       <c r="S41" s="2"/>
     </row>
-    <row r="42" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="42" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R42" s="1" t="s">
         <v>27</v>
       </c>
       <c r="S42" s="2"/>
     </row>
-    <row r="43" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="43" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R43" s="1" t="s">
         <v>28</v>
       </c>
       <c r="S43" s="2"/>
     </row>
-    <row r="44" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="44" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="H44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I44" s="2">
+        <v>0.6</v>
+      </c>
       <c r="R44" s="6">
         <f t="array" ref="R44:Y66">[1]!MF_pipe_p_atma(S34, S35, S36, S37, S38, S39, S40, S41, S42, S43)</f>
-        <v>199.04300000000001</v>
+        <v>275.262</v>
       </c>
       <c r="S44" s="6">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="T44" s="6">
         <v>10</v>
       </c>
       <c r="U44" s="6">
-        <v>199.04300000000001</v>
+        <v>275.262</v>
       </c>
       <c r="V44" s="6">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="W44" s="6">
         <v>1</v>
@@ -3960,7 +3987,13 @@
         <v>["set show_log=1 in param to show calc log"]</v>
       </c>
     </row>
-    <row r="45" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="45" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="H45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I45" s="2">
+        <v>0.86</v>
+      </c>
       <c r="R45" s="6" t="str">
         <v>p_result_atma</v>
       </c>
@@ -3986,7 +4019,13 @@
         <v>log</v>
       </c>
     </row>
-    <row r="46" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="46" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="H46" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I46" s="2">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="R46" s="6" t="str">
         <v>h,m</v>
       </c>
@@ -4012,7 +4051,13 @@
         <v>diam, mm</v>
       </c>
     </row>
-    <row r="47" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="47" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="H47" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I47" s="2">
+        <v>120</v>
+      </c>
       <c r="R47" s="6">
         <v>0</v>
       </c>
@@ -4020,7 +4065,7 @@
         <v>0</v>
       </c>
       <c r="T47" s="6">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="U47" s="6">
         <v>10</v>
@@ -4029,7 +4074,7 @@
         <v>10</v>
       </c>
       <c r="W47" s="6">
-        <v>85.471270790521913</v>
+        <v>100</v>
       </c>
       <c r="X47" s="6">
         <v>3</v>
@@ -4038,24 +4083,30 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="48" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="H48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I48" s="2">
+        <v>130</v>
+      </c>
       <c r="R48" s="6">
-        <v>147.05882352941177</v>
+        <v>138.88888888888889</v>
       </c>
       <c r="S48" s="6">
-        <v>147.05882352941177</v>
+        <v>138.88888888888889</v>
       </c>
       <c r="T48" s="6">
-        <v>36.382340650400337</v>
+        <v>24.836360057558057</v>
       </c>
       <c r="U48" s="6">
-        <v>13.676470588235293</v>
+        <v>12.666666666666666</v>
       </c>
       <c r="V48" s="6">
-        <v>13.676470588235293</v>
+        <v>12.666666666666666</v>
       </c>
       <c r="W48" s="6">
-        <v>99.24589773479029</v>
+        <v>100</v>
       </c>
       <c r="X48" s="6">
         <v>3</v>
@@ -4064,24 +4115,30 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="49" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="H49" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I49" s="2">
+        <v>80</v>
+      </c>
       <c r="R49" s="6">
-        <v>294.11764705882354</v>
+        <v>277.77777777777777</v>
       </c>
       <c r="S49" s="6">
-        <v>294.11764705882354</v>
+        <v>277.77777777777777</v>
       </c>
       <c r="T49" s="6">
-        <v>48.369222249982833</v>
+        <v>39.660912169855287</v>
       </c>
       <c r="U49" s="6">
-        <v>17.352941176470587</v>
+        <v>15.333333333333334</v>
       </c>
       <c r="V49" s="6">
-        <v>17.352941176470587</v>
+        <v>15.333333333333334</v>
       </c>
       <c r="W49" s="6">
-        <v>99.336939295122292</v>
+        <v>100</v>
       </c>
       <c r="X49" s="6">
         <v>3</v>
@@ -4090,24 +4147,30 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="50" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="H50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I50" s="2">
+        <v>1.2</v>
+      </c>
       <c r="R50" s="6">
-        <v>441.1764705882353</v>
+        <v>416.66666666666663</v>
       </c>
       <c r="S50" s="6">
-        <v>441.1764705882353</v>
+        <v>416.66666666666663</v>
       </c>
       <c r="T50" s="6">
-        <v>60.235098269119753</v>
+        <v>54.473728023011631</v>
       </c>
       <c r="U50" s="6">
-        <v>21.029411764705884</v>
+        <v>18</v>
       </c>
       <c r="V50" s="6">
-        <v>21.029411764705884</v>
+        <v>18</v>
       </c>
       <c r="W50" s="6">
-        <v>99.428325443765857</v>
+        <v>100</v>
       </c>
       <c r="X50" s="6">
         <v>3</v>
@@ -4116,417 +4179,467 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="51" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="H51" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I51" s="2">
+        <v>0.6</v>
+      </c>
       <c r="R51" s="6">
-        <v>500</v>
+        <v>555.55555555555554</v>
       </c>
       <c r="S51" s="6">
-        <v>500</v>
+        <v>555.55555555555554</v>
       </c>
       <c r="T51" s="6">
-        <v>64.947911242525024</v>
+        <v>69.274877304399666</v>
       </c>
       <c r="U51" s="6">
-        <v>22.5</v>
+        <v>20.666666666666664</v>
       </c>
       <c r="V51" s="6">
-        <v>22.5</v>
+        <v>20.666666666666664</v>
       </c>
       <c r="W51" s="6">
-        <v>99.976010537137185</v>
+        <v>100</v>
       </c>
       <c r="X51" s="6">
         <v>3</v>
       </c>
       <c r="Y51" s="6">
-        <v>72.000000000000014</v>
-      </c>
-    </row>
-    <row r="52" spans="18:25" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="H52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0</v>
+      </c>
       <c r="R52" s="6">
-        <v>588.23529411764707</v>
+        <v>694.44444444444446</v>
       </c>
       <c r="S52" s="6">
-        <v>588.23529411764707</v>
+        <v>694.44444444444446</v>
       </c>
       <c r="T52" s="6">
-        <v>72.00729056417785</v>
+        <v>84.064262054326051</v>
       </c>
       <c r="U52" s="6">
-        <v>24.705882352941178</v>
+        <v>23.333333333333332</v>
       </c>
       <c r="V52" s="6">
-        <v>24.705882352941178</v>
+        <v>23.333333333333332</v>
       </c>
       <c r="W52" s="6">
-        <v>99.959478124367394</v>
+        <v>100</v>
       </c>
       <c r="X52" s="6">
         <v>3</v>
       </c>
       <c r="Y52" s="6">
-        <v>72.000000000000014</v>
-      </c>
-    </row>
-    <row r="53" spans="18:25" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="H53" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I53" s="3" t="str">
+        <f>[1]!encode_PVT(I44,I45,I46,I47,I48,I49,I50,I51,I52)</f>
+        <v>{"gamma_gas":0.6,"gamma_oil":0.86,"gamma_wat":1.1,"rsb_m3m3":120,"pb_atma":130,"t_res_C":80,"bob_m3m3":1.2,"muob_cP":0.6,"PVT_corr_set":0}</v>
+      </c>
       <c r="R53" s="6">
-        <v>735.29411764705878</v>
+        <v>833.33333333333326</v>
       </c>
       <c r="S53" s="6">
-        <v>735.29411764705878</v>
+        <v>833.33333333333326</v>
       </c>
       <c r="T53" s="6">
-        <v>83.666494542562518</v>
+        <v>98.841955005012849</v>
       </c>
       <c r="U53" s="6">
-        <v>28.382352941176471</v>
+        <v>26</v>
       </c>
       <c r="V53" s="6">
-        <v>28.382352941176471</v>
+        <v>26</v>
       </c>
       <c r="W53" s="6">
-        <v>99.944966149157011</v>
+        <v>100</v>
       </c>
       <c r="X53" s="6">
         <v>3</v>
       </c>
       <c r="Y53" s="6">
-        <v>72.000000000000014</v>
-      </c>
-    </row>
-    <row r="54" spans="18:25" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="H54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I54" s="2">
+        <v>50</v>
+      </c>
       <c r="R54" s="6">
-        <v>882.35294117647061</v>
+        <v>972.22222222222217</v>
       </c>
       <c r="S54" s="6">
-        <v>882.35294117647061</v>
+        <v>972.22222222222217</v>
       </c>
       <c r="T54" s="6">
-        <v>95.192463420676702</v>
+        <v>113.60819486374973</v>
       </c>
       <c r="U54" s="6">
-        <v>32.058823529411768</v>
+        <v>28.666666666666664</v>
       </c>
       <c r="V54" s="6">
-        <v>32.058823529411768</v>
+        <v>28.666666666666664</v>
       </c>
       <c r="W54" s="6">
-        <v>99.938971032093662</v>
+        <v>100</v>
       </c>
       <c r="X54" s="6">
         <v>3</v>
       </c>
       <c r="Y54" s="6">
-        <v>72.000000000000014</v>
-      </c>
-    </row>
-    <row r="55" spans="18:25" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="55" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="H55" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I55" s="2">
+        <v>100</v>
+      </c>
       <c r="R55" s="6">
-        <v>1029.4117647058824</v>
+        <v>1111.1111111111111</v>
       </c>
       <c r="S55" s="6">
-        <v>1026.4705882352941</v>
+        <v>1111.1111111111111</v>
       </c>
       <c r="T55" s="6">
-        <v>106.10446404258369</v>
+        <v>128.36305394047776</v>
       </c>
       <c r="U55" s="6">
-        <v>36.191176470588239</v>
+        <v>31.333333333333332</v>
       </c>
       <c r="V55" s="6">
-        <v>36.191176470588239</v>
+        <v>31.333333333333332</v>
       </c>
       <c r="W55" s="6">
-        <v>99.972417066200819</v>
+        <v>100</v>
       </c>
       <c r="X55" s="6">
         <v>3</v>
       </c>
       <c r="Y55" s="6">
-        <v>72.000000000000014</v>
-      </c>
-    </row>
-    <row r="56" spans="18:25" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="H56" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I56" s="2">
+        <v>120</v>
+      </c>
       <c r="R56" s="6">
-        <v>1176.4705882352941</v>
+        <v>1250</v>
       </c>
       <c r="S56" s="6">
-        <v>1158.8235294117646</v>
+        <v>1250</v>
       </c>
       <c r="T56" s="6">
-        <v>116.24710999851564</v>
+        <v>143.10660666796306</v>
       </c>
       <c r="U56" s="6">
-        <v>42.147058823529413</v>
+        <v>34</v>
       </c>
       <c r="V56" s="6">
-        <v>42.147058823529413</v>
+        <v>34</v>
       </c>
       <c r="W56" s="6">
-        <v>99.970808729195454</v>
+        <v>100</v>
       </c>
       <c r="X56" s="6">
         <v>3</v>
       </c>
       <c r="Y56" s="6">
-        <v>72.000000000000014</v>
-      </c>
-    </row>
-    <row r="57" spans="18:25" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="H57" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I57" s="2">
+        <v>0</v>
+      </c>
       <c r="R57" s="6">
-        <v>1323.5294117647059</v>
+        <v>1388.8888888888889</v>
       </c>
       <c r="S57" s="6">
-        <v>1291.1764705882354</v>
+        <v>1388.8888888888889</v>
       </c>
       <c r="T57" s="6">
-        <v>126.27329543079401</v>
+        <v>157.83860705561924</v>
       </c>
       <c r="U57" s="6">
-        <v>48.102941176470587</v>
+        <v>36.666666666666664</v>
       </c>
       <c r="V57" s="6">
-        <v>48.102941176470587</v>
+        <v>36.666666666666664</v>
       </c>
       <c r="W57" s="6">
-        <v>99.968937691628938</v>
+        <v>100</v>
       </c>
       <c r="X57" s="6">
         <v>3</v>
       </c>
       <c r="Y57" s="6">
-        <v>72.000000000000014</v>
-      </c>
-    </row>
-    <row r="58" spans="18:25" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="H58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I58" s="3" t="str">
+        <f>[1]!encode_feed(I54,I55,I56,I57,I53)</f>
+        <v>{"gamma_gas":0.6,"gamma_oil":0.86,"gamma_wat":1.1,"rsb_m3m3":120,"pb_atma":130,"t_res_C":80,"bob_m3m3":1.2,"muob_cP":0.6,"PVT_corr_set":0,"q_liq_sm3day":50,"fw_perc":100,"rp_m3m3":120}</v>
+      </c>
       <c r="R58" s="6">
-        <v>1470.5882352941176</v>
+        <v>1527.7777777777778</v>
       </c>
       <c r="S58" s="6">
-        <v>1423.5294117647059</v>
+        <v>1527.7777777777778</v>
       </c>
       <c r="T58" s="6">
-        <v>136.18755283448164</v>
+        <v>172.55946291726846</v>
       </c>
       <c r="U58" s="6">
-        <v>54.058823529411761</v>
+        <v>39.333333333333329</v>
       </c>
       <c r="V58" s="6">
-        <v>54.058823529411761</v>
+        <v>39.333333333333329</v>
       </c>
       <c r="W58" s="6">
-        <v>99.966723396679313</v>
+        <v>100</v>
       </c>
       <c r="X58" s="6">
         <v>3</v>
       </c>
       <c r="Y58" s="6">
-        <v>72.000000000000014</v>
-      </c>
-    </row>
-    <row r="59" spans="18:25" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R59" s="6">
-        <v>1617.6470588235295</v>
+        <v>1666.6666666666665</v>
       </c>
       <c r="S59" s="6">
-        <v>1555.8823529411766</v>
+        <v>1666.6666666666665</v>
       </c>
       <c r="T59" s="6">
-        <v>145.9943761710272</v>
+        <v>187.26925720901431</v>
       </c>
       <c r="U59" s="6">
-        <v>60.014705882352942</v>
+        <v>41.999999999999993</v>
       </c>
       <c r="V59" s="6">
-        <v>60.014705882352942</v>
+        <v>41.999999999999993</v>
       </c>
       <c r="W59" s="6">
-        <v>99.964181680946794</v>
+        <v>100</v>
       </c>
       <c r="X59" s="6">
         <v>3</v>
       </c>
       <c r="Y59" s="6">
-        <v>72.000000000000014</v>
-      </c>
-    </row>
-    <row r="60" spans="18:25" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R60" s="6">
-        <v>1764.7058823529412</v>
+        <v>1805.5555555555554</v>
       </c>
       <c r="S60" s="6">
-        <v>1688.2352941176471</v>
+        <v>1805.5555555555554</v>
       </c>
       <c r="T60" s="6">
-        <v>155.69830991372984</v>
+        <v>201.96807608679808</v>
       </c>
       <c r="U60" s="6">
-        <v>65.970588235294116</v>
+        <v>44.666666666666657</v>
       </c>
       <c r="V60" s="6">
-        <v>65.970588235294116</v>
+        <v>44.666666666666657</v>
       </c>
       <c r="W60" s="6">
-        <v>99.961353699282455</v>
+        <v>100</v>
       </c>
       <c r="X60" s="6">
         <v>3</v>
       </c>
       <c r="Y60" s="6">
-        <v>72.000000000000014</v>
-      </c>
-    </row>
-    <row r="61" spans="18:25" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R61" s="6">
-        <v>1911.7647058823529</v>
+        <v>1944.4444444444443</v>
       </c>
       <c r="S61" s="6">
-        <v>1820.5882352941176</v>
+        <v>1944.4444444444443</v>
       </c>
       <c r="T61" s="6">
-        <v>165.28460789209592</v>
+        <v>216.65585276159905</v>
       </c>
       <c r="U61" s="6">
-        <v>71.92647058823529</v>
+        <v>47.333333333333329</v>
       </c>
       <c r="V61" s="6">
-        <v>71.92647058823529</v>
+        <v>47.333333333333329</v>
       </c>
       <c r="W61" s="6">
-        <v>99.958478906259359</v>
+        <v>100</v>
       </c>
       <c r="X61" s="6">
         <v>3</v>
       </c>
       <c r="Y61" s="6">
-        <v>72.000000000000014</v>
-      </c>
-    </row>
-    <row r="62" spans="18:25" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R62" s="6">
-        <v>2058.8235294117649</v>
+        <v>2083.3333333333335</v>
       </c>
       <c r="S62" s="6">
-        <v>1947.0588235294119</v>
+        <v>2083.3333333333335</v>
       </c>
       <c r="T62" s="6">
-        <v>174.0541851495523</v>
+        <v>231.33268489206455</v>
       </c>
       <c r="U62" s="6">
-        <v>77.617647058823536</v>
+        <v>50</v>
       </c>
       <c r="V62" s="6">
-        <v>77.617647058823536</v>
+        <v>50</v>
       </c>
       <c r="W62" s="6">
-        <v>99.955843640935882</v>
+        <v>100</v>
       </c>
       <c r="X62" s="6">
         <v>3</v>
       </c>
       <c r="Y62" s="6">
-        <v>72.000000000000014</v>
-      </c>
-    </row>
-    <row r="63" spans="18:25" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R63" s="6">
         <v>2100</v>
       </c>
       <c r="S63" s="6">
-        <v>1980</v>
+        <v>2100</v>
       </c>
       <c r="T63" s="6">
-        <v>176.40915429020524</v>
+        <v>233.09334496046432</v>
       </c>
       <c r="U63" s="6">
-        <v>79.099999999999994</v>
+        <v>50.319999999999993</v>
       </c>
       <c r="V63" s="6">
-        <v>79.099999999999994</v>
+        <v>50.319999999999993</v>
       </c>
       <c r="W63" s="6">
         <v>100</v>
       </c>
       <c r="X63" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y63" s="6">
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="64" spans="8:25" x14ac:dyDescent="0.25">
       <c r="R64" s="6">
-        <v>2205.8823529411766</v>
+        <v>2222.2222222222222</v>
       </c>
       <c r="S64" s="6">
-        <v>2064.7058823529414</v>
+        <v>2222.2222222222222</v>
       </c>
       <c r="T64" s="6">
-        <v>182.44123403347325</v>
+        <v>245.98725456824823</v>
       </c>
       <c r="U64" s="6">
-        <v>81.294117647058826</v>
+        <v>52.666666666666664</v>
       </c>
       <c r="V64" s="6">
-        <v>81.294117647058826</v>
+        <v>52.666666666666664</v>
       </c>
       <c r="W64" s="6">
         <v>100</v>
       </c>
       <c r="X64" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y64" s="6">
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="65" spans="18:25" x14ac:dyDescent="0.25">
       <c r="R65" s="6">
-        <v>2352.9411764705883</v>
+        <v>2361.1111111111109</v>
       </c>
       <c r="S65" s="6">
-        <v>2182.3529411764707</v>
+        <v>2361.1111111111109</v>
       </c>
       <c r="T65" s="6">
-        <v>190.77003183492977</v>
+        <v>260.62969555631469</v>
       </c>
       <c r="U65" s="6">
-        <v>83.647058823529406</v>
+        <v>55.333333333333329</v>
       </c>
       <c r="V65" s="6">
-        <v>83.647058823529406</v>
+        <v>55.333333333333329</v>
       </c>
       <c r="W65" s="6">
         <v>100</v>
       </c>
       <c r="X65" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y65" s="6">
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="18:25" x14ac:dyDescent="0.35">
+    <row r="66" spans="18:25" x14ac:dyDescent="0.25">
       <c r="R66" s="6">
         <v>2500</v>
       </c>
       <c r="S66" s="6">
-        <v>2300</v>
+        <v>2500</v>
       </c>
       <c r="T66" s="6">
-        <v>199.04259166672151</v>
+        <v>275.2616896761848</v>
       </c>
       <c r="U66" s="6">
-        <v>86</v>
+        <v>57.999999999999993</v>
       </c>
       <c r="V66" s="6">
-        <v>86</v>
+        <v>57.999999999999993</v>
       </c>
       <c r="W66" s="6">
         <v>100</v>
       </c>
       <c r="X66" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y66" s="6">
         <v>125</v>

</xml_diff>